<commit_message>
Atualização automática de ROSARIO_DO_SUL.xlsx
</commit_message>
<xml_diff>
--- a/ROSARIO_DO_SUL.xlsx
+++ b/ROSARIO_DO_SUL.xlsx
@@ -8,24 +8,25 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gera-fichas\Comarcas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4DF60919-26A9-49A7-97D6-147CDA9667C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C7AA3436-1864-4655-81EE-B70C49E22568}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Paineis DARQ" sheetId="6" r:id="rId1"/>
+    <sheet name="Paineis DARQ" sheetId="7" r:id="rId1"/>
     <sheet name="MATERIAIS-FORNECIDOS" sheetId="1" r:id="rId2"/>
     <sheet name="DATA-LIMITE-REQUISICOES" sheetId="2" r:id="rId3"/>
     <sheet name="CPIP" sheetId="3" r:id="rId4"/>
     <sheet name="Recolhimento x Eliminacao" sheetId="4" r:id="rId5"/>
     <sheet name="Desarquivamentos Pendentes" sheetId="5" r:id="rId6"/>
+    <sheet name="DGC" sheetId="6" r:id="rId7"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="713" uniqueCount="288">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="719" uniqueCount="292">
   <si>
     <t>Número</t>
   </si>
@@ -889,6 +890,18 @@
   </si>
   <si>
     <t>ROSÁRIO DO SUL</t>
+  </si>
+  <si>
+    <t>TEMÁTICA</t>
+  </si>
+  <si>
+    <t>PROBLEMA</t>
+  </si>
+  <si>
+    <t>MAOBRAS/MATIC</t>
+  </si>
+  <si>
+    <t>Atraso na correção do ateste.</t>
   </si>
 </sst>
 </file>
@@ -898,7 +911,7 @@
   <numFmts count="1">
     <numFmt numFmtId="165" formatCode="&quot; &quot;mmmm&quot; / &quot;yyyy"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -951,6 +964,19 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+    </font>
+    <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -965,7 +991,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1012,6 +1038,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFCE8B2"/>
         <bgColor rgb="FFFCE8B2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9D9D9"/>
+        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
     <fill>
@@ -1084,9 +1116,9 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1169,12 +1201,16 @@
     <xf numFmtId="3" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 3" xfId="1" xr:uid="{172275F9-4936-419A-A626-6F9315133CAA}"/>
+    <cellStyle name="Normal 3" xfId="1" xr:uid="{74717B82-1D3E-4B33-BFB3-9694D72E2E63}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1204,10 +1240,10 @@
         <xdr:cNvPr id="2" name="Chart1" title="Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ADFD5322-48FA-4315-BA07-D1E33E2DE276}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3948CD1B-8CE1-4A97-8DCB-AA58F772CC55}"/>
             </a:ext>
             <a:ext uri="GoogleSheetsCustomDataVersion1">
-              <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="" pictureOfChart="1"/>
+              <go:sheetsCustomData xmlns="" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:go="http://customooxmlschemas.google.com/" pictureOfChart="1"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1245,7 +1281,7 @@
         <xdr:cNvPr id="3" name="Shape 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7E99C184-C11C-4907-B2B0-0B375F815297}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EC70FF86-761A-415F-905E-1D8581986778}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1308,7 +1344,7 @@
         <xdr:cNvPr id="4" name="Shape 2" title="Desenho">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A5EAFCFD-33C6-4DCB-8706-A6E6BAFD5FFE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BD7AB156-84C4-4D99-A5BE-6E473618D61D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1327,7 +1363,7 @@
           <xdr:cNvPr id="5" name="Shape 4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FAC09115-E529-8B91-CE07-C5A7C072A0F1}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{658222CB-46E4-C8B1-A2CA-6E5CCCAE5911}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1376,7 +1412,7 @@
           <xdr:cNvPr id="6" name="Shape 5">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A3DAB910-4A90-55EB-66FB-7D2BFC6296CB}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3BD0C0FF-F178-809F-D163-6551BF0E9904}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1395,7 +1431,7 @@
             <xdr:cNvPr id="7" name="Shape 6">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8794558C-9219-6726-AD96-B8CADD5A3824}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CA79A71B-10A0-9083-1790-3B1E98A7183B}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1426,7 +1462,7 @@
             <xdr:cNvPr id="8" name="Shape 7">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{575F6E4E-A833-99D0-2106-EA50B93C0128}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3635C8E1-510C-E2B1-4B1E-4BBA98843CCA}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1457,7 +1493,7 @@
             <xdr:cNvPr id="9" name="Shape 8">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{33933C88-C1E7-4406-C77C-D758E29CF0FD}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{66F723AF-5F29-474D-064A-5F3AEDCBF9D2}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1500,7 +1536,7 @@
         <xdr:cNvPr id="10" name="image2.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{94085D89-E506-4E65-8839-9E2A4E63F193}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A9A580D2-72AA-477F-A393-F6C2242A9DF1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1538,7 +1574,7 @@
         <xdr:cNvPr id="11" name="image1.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D87D646B-1C50-4C86-A308-33922BAD75C7}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CF13F628-D0B9-405C-BBE9-C0905C0554B3}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1581,7 +1617,7 @@
         <xdr:cNvPr id="12" name="Imagem 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{83A4251E-2A62-496A-ABB7-04F30A8BD701}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{31D8336C-A710-4F8D-8705-CDDD2214BF7D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1894,7 +1930,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B991A708-CFFD-482A-9472-524F92CB70DC}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2358D59C-AF04-4E05-80B0-F816A6404EDA}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -1906,98 +1942,98 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="5" width="12.5703125" style="35"/>
-    <col min="6" max="6" width="2" style="35" customWidth="1"/>
-    <col min="7" max="16" width="13.42578125" style="35" customWidth="1"/>
-    <col min="17" max="16384" width="12.5703125" style="35"/>
+    <col min="1" max="5" width="12.5703125" style="37"/>
+    <col min="6" max="6" width="2" style="37" customWidth="1"/>
+    <col min="7" max="16" width="13.42578125" style="37" customWidth="1"/>
+    <col min="17" max="16384" width="12.5703125" style="37"/>
   </cols>
   <sheetData>
     <row r="1" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F1" s="34"/>
+      <c r="F1" s="36"/>
     </row>
     <row r="2" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F2" s="34"/>
+      <c r="F2" s="36"/>
     </row>
     <row r="3" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F3" s="34"/>
+      <c r="F3" s="36"/>
     </row>
     <row r="4" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F4" s="34"/>
+      <c r="F4" s="36"/>
     </row>
     <row r="5" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F5" s="34"/>
+      <c r="F5" s="36"/>
     </row>
     <row r="6" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F6" s="34"/>
+      <c r="F6" s="36"/>
     </row>
     <row r="7" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F7" s="34"/>
+      <c r="F7" s="36"/>
     </row>
     <row r="8" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F8" s="34"/>
+      <c r="F8" s="36"/>
     </row>
     <row r="9" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F9" s="34"/>
+      <c r="F9" s="36"/>
     </row>
     <row r="10" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F10" s="34"/>
+      <c r="F10" s="36"/>
     </row>
     <row r="11" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F11" s="34"/>
+      <c r="F11" s="36"/>
     </row>
     <row r="12" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F12" s="34"/>
+      <c r="F12" s="36"/>
     </row>
     <row r="13" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F13" s="34"/>
+      <c r="F13" s="36"/>
     </row>
     <row r="14" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F14" s="34"/>
+      <c r="F14" s="36"/>
     </row>
     <row r="15" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F15" s="34"/>
+      <c r="F15" s="36"/>
     </row>
     <row r="16" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F16" s="34"/>
+      <c r="F16" s="36"/>
     </row>
     <row r="17" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F17" s="34"/>
+      <c r="F17" s="36"/>
     </row>
     <row r="18" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F18" s="34"/>
+      <c r="F18" s="36"/>
     </row>
     <row r="19" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F19" s="34"/>
+      <c r="F19" s="36"/>
     </row>
     <row r="20" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F20" s="34"/>
+      <c r="F20" s="36"/>
     </row>
     <row r="21" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F21" s="34"/>
+      <c r="F21" s="36"/>
     </row>
     <row r="22" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F22" s="34"/>
+      <c r="F22" s="36"/>
     </row>
     <row r="23" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F23" s="34"/>
+      <c r="F23" s="36"/>
     </row>
     <row r="24" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F24" s="34"/>
+      <c r="F24" s="36"/>
     </row>
     <row r="25" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F25" s="34"/>
+      <c r="F25" s="36"/>
     </row>
     <row r="26" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F26" s="34"/>
+      <c r="F26" s="36"/>
     </row>
     <row r="27" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F27" s="34"/>
+      <c r="F27" s="36"/>
     </row>
     <row r="28" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F28" s="34"/>
+      <c r="F28" s="36"/>
     </row>
     <row r="29" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F29" s="34"/>
+      <c r="F29" s="36"/>
     </row>
   </sheetData>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -5391,4 +5427,44 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26.42578125" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" customWidth="1"/>
+    <col min="3" max="3" width="88.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="34" t="s">
+        <v>253</v>
+      </c>
+      <c r="B1" s="34" t="s">
+        <v>288</v>
+      </c>
+      <c r="C1" s="34" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="35" t="s">
+        <v>255</v>
+      </c>
+      <c r="B2" s="35" t="s">
+        <v>290</v>
+      </c>
+      <c r="C2" s="35" t="s">
+        <v>291</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>